<commit_message>
add new version of excel to the folder
</commit_message>
<xml_diff>
--- a/python_script/career_relationship.xlsx
+++ b/python_script/career_relationship.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="7575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Response" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="948">
   <si>
     <t>時間戳記</t>
   </si>
@@ -832,12 +832,13 @@
     <t>如果未來希望當啤酒品質鑑定人員，可以去考 BJCP</t>
   </si>
   <si>
-    <t>1. 具備生物化學基礎，食品化學更好
+    <t xml:space="preserve">1. 具備生物化學基礎，食品化學更好
 2. 獨立規劃並進行試驗的能力（試驗設計）
 3. 對糧食作物與農業有比一般人更深入的知識
 4. 了解一般食品工業所需的實驗儀器與檢測方法
 5. 細膩的心、活躍的腦力、強壯的臂力（可能偶爾要搬啤酒）
-6. 對啤酒產業有基本了解、酒量比一般人好、喜歡啤酒（非酗酒）</t>
+6. 對啤酒產業有基本了解、酒量比一般人好、喜歡啤酒（非酗酒）
+</t>
   </si>
   <si>
     <t>先不說啤酒，畢竟這已經是個歷史非常悠久的飲料。近代很火紅的關鍵字眼是「精釀啤酒」，去年夏天國外的精釀啤酒廠相繼慶祝他們的20週年，而公賣早已解禁十多年的台灣則是這幾年才開始風靡。精釀啤酒的訴求簡單來說是「小而美」，因為產量不大，口味上就比商業酒廠更有彈性也更多變化，給啤酒愛好者更多新奇又新鮮的選擇。而像精釀啤酒這樣的風潮，已經默默動搖到許多商業大廠的市佔率了，因此最近幾年許多國外商業大廠不是開始收購小型精釀酒廠，就是將自己的產品比照「精釀」的方式銷售。至於台灣市場，目前大概是處於天天漲停板的狀態吧！</t>
@@ -885,7 +886,8 @@
     <t>土木工程系</t>
   </si>
   <si>
-    <t>土木的背景對於之後從事營造業當然有幫助，在大學期間所學的專業知識在有關於土木的工作上都是非常重要的，但大學期間除了熟知土木專業外，還需要旁通法律的素養，像是工程採購法、民法等等，不僅可以保護自己工作安全，在與如工程規範等專業知識也可結合！</t>
+    <t xml:space="preserve">土木的背景對於之後從事營造業當然有幫助，在大學期間所學的專業知識在有關於土木的工作上都是非常重要的，但大學期間除了熟知土木專業外，還需要旁通法律的素養，像是工程採購法、民法等等，不僅可以保護自己工作安全，在與如工程規範等專業知識也可結合！
+</t>
   </si>
   <si>
     <t>營造廠、營造顧問公司、公務員</t>
@@ -909,7 +911,7 @@
     <t>國家考試</t>
   </si>
   <si>
-    <t>專業能力
+    <t xml:space="preserve">專業能力
 1.通過國家考試認定之學科能力
 2.熟稔政府採購之程序
 3.繪製或識圖能力
@@ -918,7 +920,8 @@
 人格特質
 1.善溝通與協調
 2.謹慎行事
-3.應變能力</t>
+3.應變能力
+</t>
   </si>
   <si>
     <t>1.風險高，人員流動率高
@@ -1418,8 +1421,9 @@
     <t>Chanel 精品陳列 / 布廠業務/台灣設計品牌設計師</t>
   </si>
   <si>
-    <t>務必學習好語言的部分,此產業有出差的機會,語言是基本能力
-除了有天馬行空的設計,實用性及如何完成也是這個產業要具備的基本能力！</t>
+    <t xml:space="preserve">務必學習好語言的部分,此產業有出差的機會,語言是基本能力
+除了有天馬行空的設計,實用性及如何完成也是這個產業要具備的基本能力！
+</t>
   </si>
   <si>
     <t>Yan</t>
@@ -1839,25 +1843,7 @@
     <t>中興大學</t>
   </si>
   <si>
-    <t>許雅涵</t>
-  </si>
-  <si>
-    <t>Monera1353@hotmail.com</t>
-  </si>
-  <si>
     <t>新北市政府衛生局</t>
-  </si>
-  <si>
-    <t>公部門</t>
-  </si>
-  <si>
-    <t>補習</t>
-  </si>
-  <si>
-    <t>研究助理 ，老師 ，銷售員</t>
-  </si>
-  <si>
-    <t>應具備熱情</t>
   </si>
   <si>
     <t>陳煥文</t>
@@ -2033,8 +2019,9 @@
     <t>工業設計系/設計研究所</t>
   </si>
   <si>
-    <t>大學開拓了我的視野，在台南生活也讓我開始懂得欣賞老東西和老房子，去建築系旁聽的課也讓我有機會從更遠的視角看設計的各種可能;而研究所則幫我培養解決問題和研究分析的能力。
-工業設計系教的是產品設計的邏輯和理論，在那裡可以學會動手做，實驗各種瘋狂可笑的想法，這是出社會後難再擁有的揮灑創意的機會。也因為產品設計的訓練，現在發想案子的時候，思考角度可以從2d延展到3d甚至更大的空間。</t>
+    <t xml:space="preserve">大學開拓了我的視野，在台南生活也讓我開始懂得欣賞老東西和老房子，去建築系旁聽的課也讓我有機會從更遠的視角看設計的各種可能;而研究所則幫我培養解決問題和研究分析的能力。
+工業設計系教的是產品設計的邏輯和理論，在那裡可以學會動手做，實驗各種瘋狂可笑的想法，這是出社會後難再擁有的揮灑創意的機會。也因為產品設計的訓練，現在發想案子的時候，思考角度可以從2d延展到3d甚至更大的空間。
+</t>
   </si>
   <si>
     <t>ＵＸ設計師、攝影師、產品設計師</t>
@@ -2121,11 +2108,12 @@
     <t>相關科系(都市計畫、景觀、防災、建築...)之學/碩士畢業者，入行無須通過任何考試/證照，但日後若想自行成立公司或事務所，都市計畫技師證照是基本條件。</t>
   </si>
   <si>
-    <t>此行業之制式成果為報告書及圖面，單就達成這兩項成果所需之技術能力而言，基本文書處理及進階製圖能力(地理資訊系統、AutoCAD)是必須的。
+    <t xml:space="preserve">此行業之制式成果為報告書及圖面，單就達成這兩項成果所需之技術能力而言，基本文書處理及進階製圖能力(地理資訊系統、AutoCAD)是必須的。
 然空間規劃之範疇其實包山包海，尺度大至國家、小至社區，其牽涉專業領域之廣難以用短短文字表達，然若細究案件執行過程，所需專業能力可大略分為下列幾點：
 1.需有理解法條內容之能力(國土計畫法、都市計畫法、都市更新條例...等)
 2.能了解並運用各個尺度空間(國土-區域-都市-社區)與各專業領域(人口、交通、產業、水利、測量、估價...等)相對應之分析方法，並能有條理地統整、歸納各項分析結果後提出具體之規畫方案。
-3.空間規劃者是政府與民眾與土地、空間議題上之橋梁(專業第三方)，因此應具  備與人(民眾、業主、行政機關)溝通斡旋之對應能力。</t>
+3.空間規劃者是政府與民眾與土地、空間議題上之橋梁(專業第三方)，因此應具  備與人(民眾、業主、行政機關)溝通斡旋之對應能力。
+</t>
   </si>
   <si>
     <t>單以私部門而言，都市規劃產業現況主要可分為傳統規劃與非傳統規劃兩類型，傳統規劃多以各個都市計畫區之通盤檢討案、個案變更案，以及私人委託之非都市土地開發案等為主要案源；非傳統規劃則會以各類型的可行性研究、都市再生規劃、文化資產保存、社區規劃、都市設計策略...等。
@@ -2238,7 +2226,8 @@
     <t>就讀生物相關科系所即可，目前略可粗分三組:生態環境組、生物資訊組、生物醫學組。依各實驗室屬性不同需要不同專長。目前所屬的癌症轉譯實驗室為生物醫學組，主探討癌細胞訊息調控生長機轉與臨床實證，需具備基礎細胞生物學及分子生物學相關知識，取得碩士學位者佳，因具備獨立實驗操作能力(ex:細胞無菌培養、分生實驗、動物實驗)。另外實驗設計分析、論文搜尋閱讀撰寫、讀懂實驗操作手冊(protocol、datasheet)、化學溶液與藥品單位換算配製也是必備能力。常需與老闆開會討論實驗結果(本實驗室為每天一對一有效率討論)。對實驗有相當熱枕(覺得實驗就像是遊戲般有趣)為佳，較能挺過失敗低潮期。</t>
   </si>
   <si>
-    <t>因應國衛院、科技部、農委會等相關政府研究計畫補助獎勵，目前研究助理的角色仍是不可或缺的。但工作穩定度還是得視所屬老闆取得計畫補助能力。待過學校與醫院的我，目前覺得醫院研究助理相對穩定，醫生的計畫來源較多元(除了科技、國衛院、醫院內外計畫與藥廠合作計畫)，資金充足。但也不是每個醫師實驗室都有如此優渥環境，所以跟對一個認真打拼的醫生老闆(或是學校教授)還是非常重要的。雖然常有人對於年簽計畫合約感到質疑不安(醫生護士的工作約也是年簽)，但本人認為，只要努力執行計畫實驗，做出好結果讓老闆能順利取得計畫不也是魚幫水、水幫魚嗎?</t>
+    <t xml:space="preserve">因應國衛院、科技部、農委會等相關政府研究計畫補助獎勵，目前研究助理的角色仍是不可或缺的。但工作穩定度還是得視所屬老闆取得計畫補助能力。待過學校與醫院的我，目前覺得醫院研究助理相對穩定，醫生的計畫來源較多元(除了科技、國衛院、醫院內外計畫與藥廠合作計畫)，資金充足。但也不是每個醫師實驗室都有如此優渥環境，所以跟對一個認真打拼的醫生老闆(或是學校教授)還是非常重要的。雖然常有人對於年簽計畫合約感到質疑不安(醫生護士的工作約也是年簽)，但本人認為，只要努力執行計畫實驗，做出好結果讓老闆能順利取得計畫不也是魚幫水、水幫魚嗎?
+</t>
   </si>
   <si>
     <t>大學:生物科技學系。碩班:生命科學系所。</t>
@@ -2574,7 +2563,8 @@
 （ps.在書店工作，什麼類型的客人都絕對遇的到，所以高EQ以及說話藝術也非常非常非常非常重要）</t>
   </si>
   <si>
-    <t>在閱讀力及閱讀品質趨漸下滑的社會裡，不論是寫一本書、出版一本書甚至再賣掉一本書，都不會是一件容易的事情。既苦也甘。</t>
+    <t xml:space="preserve">在閱讀力及閱讀品質趨漸下滑的社會裡，不論是寫一本書、出版一本書甚至再賣掉一本書，都不會是一件容易的事情。既苦也甘。
+</t>
   </si>
   <si>
     <t>嘉義大學生農系</t>
@@ -2653,6 +2643,366 @@
   </si>
   <si>
     <t>崑山科大</t>
+  </si>
+  <si>
+    <t>徐嘉偉</t>
+  </si>
+  <si>
+    <t>peterfr073615521@gmail.com</t>
+  </si>
+  <si>
+    <t>專任助理</t>
+  </si>
+  <si>
+    <t>國立臺北大學</t>
+  </si>
+  <si>
+    <t>善於溝通、有耐心、對所屬領域有熱忱、不排斥繁雜的行政流程、樂於學習</t>
+  </si>
+  <si>
+    <t>學校的計畫專任助理通常是一年一聘，視該計畫持續多久，以及經費多寡來決定是否續聘，因此此工作長期下來，穩定性較低，但由於工時、薪水較為固定，且休息時間較多，很適合想彈性安排時間，或有志於升學、應考的求職者應徵。</t>
+  </si>
+  <si>
+    <t>工業與資訊管理學系</t>
+  </si>
+  <si>
+    <t>因為我的工作之一是協助學校的數位學習推廣，所以跟資管有一點點相關，但關聯性不大。我主要都是透過閱讀、實務等累積經驗</t>
+  </si>
+  <si>
+    <t>程式設計師、品管人員、軟體相關等等</t>
+  </si>
+  <si>
+    <t>李昀蓁</t>
+  </si>
+  <si>
+    <t>fuples@hotmail.com</t>
+  </si>
+  <si>
+    <t>建築師</t>
+  </si>
+  <si>
+    <t>東 環境・ 建築研究所</t>
+  </si>
+  <si>
+    <t>建築師，日文檢定（因於日本工作）</t>
+  </si>
+  <si>
+    <t>建築專業能力，耐心與持續度</t>
+  </si>
+  <si>
+    <t>台灣民眾普遍美感不足，不尊重專業。設計師與業主的概念有相當大的出入，導致設計師無法完整呈現自己的設計，要遇到好的業主非常困難。
+政府也不重視專業，導致許多公共工程施工品質不佳，設計更是令人堪憂。</t>
+  </si>
+  <si>
+    <t>建築所</t>
+  </si>
+  <si>
+    <t>建築專業知識，電腦繪圖軟體使用能力，設計創造能力</t>
+  </si>
+  <si>
+    <t>建築師事務所，台北都發局，室內設計公司</t>
+  </si>
+  <si>
+    <t>要進建築圈需要有相當大的覺悟，工作時不像學生時期可以無拘無束的做設計。會遇到許多法規上的限制，業主的堅持，經費不足等等相當實際面的問題。
+但相對的，突破這些侷限做出自己想要的設計相當有成就感。
+痛苦會過去，美會留下。
+但建築圈的痛苦有點長，留下來的東西有時候因為眾多限制而不美了。
+各位加油</t>
+  </si>
+  <si>
+    <t>逢甲建築系/成大建研所</t>
+  </si>
+  <si>
+    <t>林彥成</t>
+  </si>
+  <si>
+    <t>breaking0215@hotmail.com</t>
+  </si>
+  <si>
+    <t>Front-end developer</t>
+  </si>
+  <si>
+    <t>北宸科技</t>
+  </si>
+  <si>
+    <t>不需要XD</t>
+  </si>
+  <si>
+    <t>喜歡Web相關領域知識，了解並進入Open source 的領域，快點開Github帳號吧XD</t>
+  </si>
+  <si>
+    <t>GIS 相關不是很賺錢 0.0</t>
+  </si>
+  <si>
+    <t>工程科學系</t>
+  </si>
+  <si>
+    <t>計算機相關領域的能力吧XD 不過還是建議修一些資工系的課補強~</t>
+  </si>
+  <si>
+    <t>半導體業, IC設計業, 一般軟體業</t>
+  </si>
+  <si>
+    <t>坑很大(無誤XD) 另外有機會就早點出國吧~</t>
+  </si>
+  <si>
+    <t>工程科學所(資訊組)</t>
+  </si>
+  <si>
+    <t>許芷綾</t>
+  </si>
+  <si>
+    <t>loverlovertw2@hotmail.com</t>
+  </si>
+  <si>
+    <t>衛生所</t>
+  </si>
+  <si>
+    <t>與民眾的應對,法規熟悉度,機警並靈活地面對不同的人事物</t>
+  </si>
+  <si>
+    <t>缺乏人力,照目前年金改革方向,未來福利減少(其實目前福利也沒有說特好</t>
+  </si>
+  <si>
+    <t>醫技系</t>
+  </si>
+  <si>
+    <t>因透過高普考考試近來公職,在考科中僅有微生物以及生物統計對考試有幫助,至於應對方方面,在進入職場後透過每一次互動,調整自己的態度與處理方式</t>
+  </si>
+  <si>
+    <t>教授,醫檢師,生物科技公司上班</t>
+  </si>
+  <si>
+    <t>在人民至上,公務人員是民眾的員工此風氣下,進入公職需要面對許多形形色色的民眾,調整自己的態度以求不卑不亢,對態度不好的民眾不委屈求全,對態度好的民眾不擺出'我是官'的態度,在情與法之間求一平衡點</t>
+  </si>
+  <si>
+    <t>廖智群</t>
+  </si>
+  <si>
+    <t>Eagle_thomas@hotmail.com</t>
+  </si>
+  <si>
+    <t>副機師</t>
+  </si>
+  <si>
+    <t>中華航空</t>
+  </si>
+  <si>
+    <t>英檢 飛行執照</t>
+  </si>
+  <si>
+    <t>樂觀開朗 抗壓度高</t>
+  </si>
+  <si>
+    <t>高專業 高報酬</t>
+  </si>
+  <si>
+    <t>航太系</t>
+  </si>
+  <si>
+    <t>對工作內容相對熟悉，部分專業內容與學校學科相同</t>
+  </si>
+  <si>
+    <t>科技業工程師  漢翔工程師  中科院工程師</t>
+  </si>
+  <si>
+    <t>成大航太所</t>
+  </si>
+  <si>
+    <t>曾正偉</t>
+  </si>
+  <si>
+    <t>s0337@yfy.com</t>
+  </si>
+  <si>
+    <t>工程師</t>
+  </si>
+  <si>
+    <t>永豐餘工業用紙公司新屋廠</t>
+  </si>
+  <si>
+    <t>需修習熱力學、熱傳學相關課程</t>
+  </si>
+  <si>
+    <t>除了需修習熱力學、熱傳學相關課程之外，平時尚需自行研讀化學反應、流體化床反應器、電力儀表、邏輯控制、鍋爐操作、機械裝修等等各式各樣的專業知識，需要具備主動積極、熱心學習的態度、和同儕前輩溝通討論、團隊合作的能力、在高階主管面前簡報說明工作進度、面臨困難、未來展望、爭取經費的口條；目前本公司主要以造紙餘下之紙渣-塑膠片混合料作為裂解產製工業重油之原料，將來或將結合生質物汽化以及沼氣發電，成為再生能源的中堅。</t>
+  </si>
+  <si>
+    <t>目前本公司主要以造紙餘下之紙渣-塑膠片混合料作為裂解產製工業重油之原料，將來或將結合生質物汽化以及沼氣發電，成為再生能源的中堅。本部門目前直隸永豐餘集團策略長室之能資源再利用平臺，主掌永豐餘集團臺灣、大陸、越南數十個廠區的事故維護、能源諮詢和原料/技術交流，現在亦與工研院、中興、中央、元智、中原等學校/機構有各項合作計畫；目前在桃園新屋建有5噸試驗廠，近期將開始擴充為日進量50噸之商業流體化床裂解廠，為臺灣綠能努力。</t>
+  </si>
+  <si>
+    <t>國立成功大學資源工程學系</t>
+  </si>
+  <si>
+    <t>就讀科系與工作內容有關，僅限於入門的基礎能力：包括熱力學、熱傳學知識、流體化床的性質、快速熱裂解產製重油製程、基本化學分析等等; 但大部分工作內容和就讀科系較為無關，主要是以自修或請教前輩培養相關能力，像是：工廠儀器設備面臨突然跳電時，如何透過檢測電力儀表快速獲知故障的發生點、設備運作時藉由對其邏輯控制的認知簡化操作程序、時間、成本等等，學會鍋爐操作、參數調控維持製程的穩定、機械配件的安裝修飾、團隊合作的能力、簡報的技巧、爭取經費的口條等等，都是要透過在職場一次又一次不斷的磨鍊，才能漸漸達到的，得之不易。</t>
+  </si>
+  <si>
+    <t>臺積電設備工程師、鴻海精密工程師、東元電機機構工程師</t>
+  </si>
+  <si>
+    <t>未來若是想從事這個工作可能需要以自修或請教前輩培養相關能力，皆要透過在職場一次又一次不斷的磨鍊，才能臻於完成。</t>
+  </si>
+  <si>
+    <t>國立中央大學能源工程研究所</t>
+  </si>
+  <si>
+    <t>吳泓頡</t>
+  </si>
+  <si>
+    <t>za0912938473@hotmail.com</t>
+  </si>
+  <si>
+    <t>新聞編譯</t>
+  </si>
+  <si>
+    <t>亞洲衛星電視台</t>
+  </si>
+  <si>
+    <t>基本上不太需要</t>
+  </si>
+  <si>
+    <t>對國際新聞有熱忱，願意接觸者</t>
+  </si>
+  <si>
+    <t>新聞業相對發展性比較死，但是培養出新聞能力，有機會成為名主播或記者</t>
+  </si>
+  <si>
+    <t>其實國際新聞這塊，說有關也有關，但是唯一關聯就是英語能力會比其他科系有點優勢，最重要還是進去後肯不肯學，我自己大學對這塊也完全不懂，很多能力都是進去後，請教前輩的</t>
+  </si>
+  <si>
+    <t>老師、公務員、行銷</t>
+  </si>
+  <si>
+    <t>要能忍受寫稿時自己作業的寂寞，要學會和剪接打交通，最重要的是，多參考其他人寫的新聞，從中學習用字、過音、畫面感</t>
+  </si>
+  <si>
+    <t>吳佳芬</t>
+  </si>
+  <si>
+    <t>cutechiafen@yahoo.com.tw</t>
+  </si>
+  <si>
+    <t>副管理師</t>
+  </si>
+  <si>
+    <t>寶成工業股份有限公司</t>
+  </si>
+  <si>
+    <t>需具備細心及耐心，也需要替其他同仁及員工服務，是一份例行性但也是不可或缺的工作</t>
+  </si>
+  <si>
+    <t>極為良好</t>
+  </si>
+  <si>
+    <t>應用外語系</t>
+  </si>
+  <si>
+    <t>從中學習並培養其能力</t>
+  </si>
+  <si>
+    <t>創業、教師及公司行業工作</t>
+  </si>
+  <si>
+    <t>細心及耐心，才有辦法勝任這一份工作</t>
+  </si>
+  <si>
+    <t>美國康寇迪亞TESOL研究所</t>
+  </si>
+  <si>
+    <t>何諺錡</t>
+  </si>
+  <si>
+    <t>yenchiho@microsoft.com</t>
+  </si>
+  <si>
+    <t>大中華區微軟雲市場經理 雲計算與企業事業部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft </t>
+  </si>
+  <si>
+    <t>English Proficiency Tests, Programming Skill</t>
+  </si>
+  <si>
+    <t>對任何事物保有高度好奇心與熱忱，並快速學習實用的能力、組織協調能力、邏輯推演能力、宏觀視野以及實際動手操作的實作能力，必須能夠快速學習快速實作接著快速理解與快速除錯並應用</t>
+  </si>
+  <si>
+    <t>公有雲是高度競爭且快速發展的行業，也是改變未來世界樣貌的重要產業，是資訊產業中的一塊非常有趣的領域，其應用層面涵蓋幾乎所有領域，因此也需要對於各產業都有足夠的認知及興趣，才能協助客戶創造最大價值</t>
+  </si>
+  <si>
+    <t>程式設計、產品規劃與時程安排、基本對於計算機的認知以及應用開發都相當重要，此外團隊合作以及領導能力也是重要內容。
+最重要的是結識各科系朋友，補足對於各領域的基礎並推導洞見</t>
+  </si>
+  <si>
+    <t>LinkedIn、台積電、Intel</t>
+  </si>
+  <si>
+    <t>微軟是一間歷史悠久的資訊公司，有非常大量的資源挹注在科技與產品技術等等的研發上，舉凡設計、生物科學、資料科學、電腦科學、人力資源、社會公益、法務、文書、行銷、銷售等，有非常多產品線以及各種職業部門能選擇，因此各行各業的菁英都能在這間公司找到適合的位子，並且一起創造更多良好的使用體驗給我們的合作夥伴與客戶！</t>
+  </si>
+  <si>
+    <t>王祥宇</t>
+  </si>
+  <si>
+    <t>limitnick@hotmail.com</t>
+  </si>
+  <si>
+    <t>android工程師</t>
+  </si>
+  <si>
+    <t>Mattel</t>
+  </si>
+  <si>
+    <t>科系不重要，但要碩士畢業，會寫JAVA跟android，英文能力中上，邏輯能力要強，習慣無理的加班，程式語言會越多越好，因為永遠無法預測科技潮流的走向</t>
+  </si>
+  <si>
+    <t>在國外很賺，在台灣餓不死但也賺不了大錢，有機會就離開台灣吧</t>
+  </si>
+  <si>
+    <t>通訊與導航工程學系</t>
+  </si>
+  <si>
+    <t>碩班找到對的老師帶你上天堂</t>
+  </si>
+  <si>
+    <t>中華電信工程師</t>
+  </si>
+  <si>
+    <t>真的有興趣再來</t>
+  </si>
+  <si>
+    <t>臺灣海洋大學 碩士班</t>
+  </si>
+  <si>
+    <t>Heidi</t>
+  </si>
+  <si>
+    <t>yuching268@gmail.com</t>
+  </si>
+  <si>
+    <t>室內設計師</t>
+  </si>
+  <si>
+    <t>成舍室內設計</t>
+  </si>
+  <si>
+    <t>專業能力方面，要熟悉繪圖軟體，例如AutoCAD, sketch up, Adobe系列等；也要有繪製細部施工圖的能力
+人格特質的部分，最重要的，應該是要懂得傾聽他人需求，並擁有良好的溝通能力；從事這個行業需要大量的與他人協商、討論，並有良好的邏輯</t>
+  </si>
+  <si>
+    <t>只能說很血汗，責任制，假日不一定都能放到假。</t>
+  </si>
+  <si>
+    <t>建築系</t>
+  </si>
+  <si>
+    <t>空間概念、軟體上的操作、施工圖的繪製等，都是在就學期間能培養的能力
+對於美感、設計感的敏感度，也都是在就讀相關科系時能培養出來的</t>
+  </si>
+  <si>
+    <t>建築設計、室內設計、工程結構設計</t>
+  </si>
+  <si>
+    <t>認真覺得要有足夠的熱情或興趣才有辦法持續燃燒，
+否則只會覺得工作很操很累，很不值得為此消耗自己的時間與健康</t>
   </si>
 </sst>
 </file>
@@ -3034,11 +3384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U73"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3046,8 +3396,7 @@
     <col min="1" max="8" width="21.5703125" customWidth="1"/>
     <col min="9" max="9" width="54.85546875" customWidth="1"/>
     <col min="10" max="18" width="21.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" customWidth="1"/>
+    <col min="19" max="20" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1">
@@ -5914,38 +6263,38 @@
       </c>
     </row>
     <row r="49" spans="1:20">
-      <c r="A49" s="5">
-        <v>42559.058615891205</v>
+      <c r="A49" s="10">
+        <v>42559.089771979168</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>579</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>55</v>
+        <v>581</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>79</v>
+        <v>582</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>68</v>
@@ -5954,16 +6303,16 @@
         <v>79</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="S49" s="1" t="s">
         <v>35</v>
@@ -5973,38 +6322,38 @@
       </c>
     </row>
     <row r="50" spans="1:20">
-      <c r="A50" s="10">
-        <v>42559.089771979168</v>
+      <c r="A50" s="5">
+        <v>42559.104210173609</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>579</v>
+        <v>591</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>74</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>587</v>
+        <v>87</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>68</v>
@@ -6013,16 +6362,16 @@
         <v>79</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="S50" s="1" t="s">
         <v>35</v>
@@ -6032,56 +6381,56 @@
       </c>
     </row>
     <row r="51" spans="1:20">
-      <c r="A51" s="5">
-        <v>42559.104210173609</v>
+      <c r="A51" s="10">
+        <v>42559.292962789354</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>87</v>
+        <v>333</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>68</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>603</v>
+        <v>576</v>
       </c>
       <c r="S51" s="1" t="s">
         <v>35</v>
@@ -6091,315 +6440,309 @@
       </c>
     </row>
     <row r="52" spans="1:20">
-      <c r="A52" s="10">
-        <v>42559.292962789354</v>
+      <c r="A52" s="5">
+        <v>42559.353507222222</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>333</v>
+        <v>147</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>68</v>
+        <v>613</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>576</v>
+        <v>616</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>36</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:20">
-      <c r="A53" s="5">
-        <v>42559.353507222222</v>
+      <c r="A53" s="10">
+        <v>42559.465064039352</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>147</v>
+        <v>23</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>620</v>
+        <v>624</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>625</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>66</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>210</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:20">
-      <c r="A54" s="10">
-        <v>42559.465064039352</v>
+    <row r="54" spans="1:20" ht="18">
+      <c r="A54" s="5">
+        <v>42559.534836805557</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>101</v>
+        <v>174</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>23</v>
+        <v>333</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="S54" s="1" t="s">
-        <v>66</v>
+        <v>638</v>
+      </c>
+      <c r="S54" s="8" t="s">
+        <v>357</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>67</v>
+        <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="18">
-      <c r="A55" s="5">
-        <v>42559.534836805557</v>
+    <row r="55" spans="1:20">
+      <c r="A55" s="10">
+        <v>42559.607200081024</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>333</v>
+        <v>87</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>640</v>
+        <v>68</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="S55" s="8" t="s">
-        <v>357</v>
+        <v>576</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>369</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:20">
-      <c r="A56" s="10">
-        <v>42559.607200081024</v>
+      <c r="A56" s="5">
+        <v>42559.61126416667</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>87</v>
+        <v>652</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>68</v>
+        <v>655</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>576</v>
+        <v>657</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>36</v>
+        <v>658</v>
       </c>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" ht="18">
       <c r="A57" s="5">
-        <v>42559.61126416667</v>
+        <v>42559.61152622685</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>23</v>
@@ -6408,346 +6751,349 @@
         <v>74</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>662</v>
+        <v>667</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>669</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="S57" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="S57" s="8" t="s">
+        <v>357</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>664</v>
+        <v>369</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="18">
+    <row r="58" spans="1:20">
       <c r="A58" s="5">
-        <v>42559.61152622685</v>
+        <v>42559.613134814819</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S58" s="8" t="s">
-        <v>357</v>
+        <v>681</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>369</v>
+        <v>658</v>
       </c>
     </row>
     <row r="59" spans="1:20">
-      <c r="A59" s="5">
-        <v>42559.613134814819</v>
+      <c r="A59" s="10">
+        <v>42561.594228009257</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>680</v>
+        <v>547</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>687</v>
+        <v>69</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>664</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:20">
       <c r="A60" s="10">
-        <v>42561.594228009257</v>
+        <v>42561.938788935186</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>547</v>
+        <v>333</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="N60" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>69</v>
+        <v>702</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>169</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:20">
-      <c r="A61" s="10">
-        <v>42561.938788935186</v>
+      <c r="A61" s="5">
+        <v>42562.984602187498</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>333</v>
+        <v>707</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>702</v>
+        <v>708</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>704</v>
+        <v>519</v>
       </c>
       <c r="N61" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>708</v>
+        <v>129</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="T61" s="6" t="s">
-        <v>36</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:20">
       <c r="A62" s="5">
-        <v>42562.984602187498</v>
+        <v>42563.44498255787</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>711</v>
+        <v>159</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>519</v>
+        <v>719</v>
       </c>
       <c r="N62" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>129</v>
+        <v>722</v>
       </c>
       <c r="S62" s="1" t="s">
         <v>50</v>
       </c>
       <c r="T62" s="6" t="s">
-        <v>186</v>
+        <v>658</v>
       </c>
     </row>
     <row r="63" spans="1:20">
-      <c r="A63" s="5">
-        <v>42563.44498255787</v>
+      <c r="A63" s="10">
+        <v>42564.928872083328</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>159</v>
+        <v>682</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>23</v>
@@ -6756,349 +7102,352 @@
         <v>101</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>725</v>
+        <v>185</v>
       </c>
       <c r="N63" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>727</v>
+        <v>730</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>731</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>728</v>
+        <v>69</v>
       </c>
       <c r="S63" s="1" t="s">
         <v>50</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>664</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:20">
       <c r="A64" s="10">
-        <v>42564.928872083328</v>
+        <v>42573.910546678242</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>688</v>
+        <v>514</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>185</v>
+        <v>738</v>
       </c>
       <c r="N64" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>69</v>
+        <v>742</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:20">
       <c r="A65" s="10">
-        <v>42573.910546678242</v>
+        <v>42573.954040266202</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>514</v>
+        <v>745</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="N65" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="R65" s="1" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="T65" s="6" t="s">
-        <v>36</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" ht="12.75">
       <c r="A66" s="10">
-        <v>42573.954040266202</v>
+        <v>42573.997384224538</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="N66" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>759</v>
+        <v>764</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="S66" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="T66" s="6" t="s">
+      <c r="T66" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="12.75">
+    <row r="67" spans="1:20">
       <c r="A67" s="10">
-        <v>42573.997384224538</v>
+        <v>42574.891032395833</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>763</v>
+        <v>768</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>756</v>
+        <v>773</v>
       </c>
       <c r="N67" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>169</v>
+        <v>66</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:20">
       <c r="A68" s="10">
-        <v>42574.891032395833</v>
+        <v>42576.861528761576</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c r="N68" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="R68" s="1" t="s">
-        <v>783</v>
+        <v>627</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:20">
       <c r="A69" s="10">
-        <v>42576.861528761576</v>
+        <v>42576.863141134258</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>23</v>
@@ -7107,146 +7456,149 @@
         <v>101</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>788</v>
+        <v>333</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>633</v>
+        <v>25</v>
+      </c>
+      <c r="S69" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>169</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:20">
-      <c r="A70" s="10">
-        <v>42576.863141134258</v>
+      <c r="A70" s="12">
+        <v>42576.984813807867</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>101</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>333</v>
+        <v>79</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="P70" s="1" t="s">
-        <v>803</v>
+        <v>159</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>25</v>
+        <v>808</v>
       </c>
       <c r="S70" s="1" t="s">
         <v>35</v>
       </c>
       <c r="T70" s="6" t="s">
-        <v>36</v>
+        <v>267</v>
       </c>
     </row>
     <row r="71" spans="1:20">
       <c r="A71" s="12">
-        <v>42576.984813807867</v>
+        <v>42580.983355706019</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>101</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="P71" s="1" t="s">
-        <v>159</v>
+        <v>817</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
       <c r="R71" s="1" t="s">
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="S71" s="1" t="s">
         <v>35</v>
@@ -7257,22 +7609,22 @@
     </row>
     <row r="72" spans="1:20">
       <c r="A72" s="12">
-        <v>42580.983355706019</v>
+        <v>42627.902591307866</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>23</v>
@@ -7281,96 +7633,680 @@
         <v>101</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>333</v>
+        <v>87</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>825</v>
+        <v>830</v>
       </c>
       <c r="S72" s="1" t="s">
-        <v>35</v>
+        <v>182</v>
       </c>
       <c r="T72" s="6" t="s">
-        <v>267</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:20">
       <c r="A73" s="12">
-        <v>42627.902591307866</v>
+        <v>42781.633855810185</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="P73" s="1" t="s">
-        <v>834</v>
-      </c>
-      <c r="Q73" s="1" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="R73" s="1" t="s">
-        <v>836</v>
+        <v>25</v>
       </c>
       <c r="S73" s="1" t="s">
         <v>182</v>
       </c>
       <c r="T73" s="6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="18">
+      <c r="A74" s="12">
+        <v>42781.748011655094</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="S74" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
+      <c r="A75" s="12">
+        <v>42781.845392326388</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="S75" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T75" s="6" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
+      <c r="A76" s="12">
+        <v>42782.480274224537</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="R76" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="S76" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T76" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
+      <c r="A77" s="12">
+        <v>42782.826721481484</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="P77" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="S77" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T77" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
+      <c r="A78" s="12">
+        <v>42783.008120081024</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="P78" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="R78" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="S78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T78" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
+      <c r="A79" s="12">
+        <v>42784.594061342592</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="N79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="P79" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T79" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
+      <c r="A80" s="12">
+        <v>42784.6041290625</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="N80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="S80" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T80" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
+      <c r="A81" s="12">
+        <v>42788.002158715273</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S81" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T81" s="6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
+      <c r="A82" s="12">
+        <v>42809.976260057869</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="S82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T82" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" ht="18">
+      <c r="A83" s="12">
+        <v>42809.988140775458</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S83" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="T83" s="6" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>